<commit_message>
pretest and scan instructions update
</commit_message>
<xml_diff>
--- a/fMRI experiment/psychopy code/listening_instructions.xlsx
+++ b/fMRI experiment/psychopy code/listening_instructions.xlsx
@@ -1,6 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>instructions</t>
   </si>
@@ -29,6 +30,12 @@
   </si>
   <si>
     <t>Please “simulate” this job while you listen to the story that follows.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Even if we do not give you a perspective for some of them, please listen to all of the stories carefully. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to be as still as possible during the scan, especially as you are listening to the stories. </t>
   </si>
   <si>
     <t>Before you begin, we will go over how to use the button box:</t>
@@ -1362,7 +1369,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1449,7 +1456,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" ht="92.35" customHeight="1">
+    <row r="8" ht="56.35" customHeight="1">
       <c r="A8" t="s" s="7">
         <v>7</v>
       </c>
@@ -1460,8 +1467,10 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="10"/>
+    <row r="9" ht="56.35" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>8</v>
+      </c>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1469,8 +1478,10 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="10"/>
+    <row r="10" ht="92.35" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>9</v>
+      </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -1586,6 +1597,24 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
+    <row r="23" ht="20.35" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" ht="20.35" customHeight="1">
+      <c r="A24" s="10"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>